<commit_message>
tempo para escrita aumentado 1500
</commit_message>
<xml_diff>
--- a/Planilhas Excel/Conferencia_de_valores.xlsx
+++ b/Planilhas Excel/Conferencia_de_valores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3beaf518c581d7d9/Documentos/GitHub/Fuzzy_Logic_2_Controller/Planilhas Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{E7D119CA-9AE4-4C47-BE3C-22F746B05797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D699534A-E0D3-436A-91A4-B4BA2B590CA6}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{E7D119CA-9AE4-4C47-BE3C-22F746B05797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68D97908-D838-493D-80F2-F30BA6CC3C0D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{377A5F18-558A-4A8F-B21A-CB5653200D67}"/>
+    <workbookView minimized="1" xWindow="3660" yWindow="2475" windowWidth="21600" windowHeight="11295" xr2:uid="{377A5F18-558A-4A8F-B21A-CB5653200D67}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -582,7 +582,7 @@
   <dimension ref="A1:AD14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,14 +714,14 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B3" s="1">
-        <v>128</v>
+        <v>216</v>
       </c>
       <c r="E3" s="2">
         <f>IF($A$3&lt;S3,0,IF($A$3&lt;S4,255*($A$3-S3)/(S4-S3),IF($A$3&lt;S5,255,IF($A$3&lt;S6,255*(S6-$A$3)/(S6-S5),0))))</f>
-        <v>8.0952380952380949</v>
+        <v>48.571428571428569</v>
       </c>
       <c r="F3" s="2">
         <f>IF($A$3&lt;T3,0,IF($A$3&lt;T4,255*($A$3-T3)/(T4-T3),IF($A$3&lt;T5,255,IF($A$3&lt;T6,255*(T6-$A$3)/(T6-T5),0))))</f>
@@ -733,19 +733,19 @@
       </c>
       <c r="H3" s="2">
         <f>IF($B$3&lt;V3,0,IF($B$3&lt;V4,255*($B$3-V3)/(V4-V3),IF($B$3&lt;V5,255,IF($B$3&lt;V6,255*(V6-$B$3)/(V6-V5),0))))</f>
-        <v>71.83098591549296</v>
+        <v>0</v>
       </c>
       <c r="I3" s="2">
         <f>IF($B$3&lt;W3,0,IF($B$3&lt;W4,255*($B$3-W3)/(W4-W3),IF($B$3&lt;W5,255,IF($B$3&lt;W6,255*(W6-$B$3)/(W6-W5),0))))</f>
-        <v>255</v>
+        <v>122.11267605633803</v>
       </c>
       <c r="J3" s="4">
         <f>IF($B$3&lt;X3,0,IF($B$3&lt;X4,255*($B$3-X3)/(X4-X3),IF($B$3&lt;X5,255,IF($B$3&lt;X6,255*(X6-$B$3)/(X6-X5),0))))</f>
-        <v>0</v>
+        <v>208.63636363636363</v>
       </c>
       <c r="K3" s="3">
         <f>IF($A$3&lt;Y3,0,IF($A$3&lt;Y4,255*($A$3-Y3)/(Y4-Y3),IF($A$3&lt;Y5,255,IF($A$3&lt;Y6,255*(Y6-$A$3)/(Y6-Y5),0))))</f>
-        <v>0</v>
+        <v>22.767857142857142</v>
       </c>
       <c r="L3" s="2">
         <f>IF($A$3&lt;Z3,0,IF($A$3&lt;Z4,255*($A$3-Z3)/(Z4-Z3),IF($A$3&lt;Z5,255,IF($A$3&lt;Z6,255*(Z6-$A$3)/(Z6-Z5),0))))</f>
@@ -757,15 +757,15 @@
       </c>
       <c r="N3" s="2">
         <f>IF($B$3&lt;AB3,0,IF($B$3&lt;AB4,255*($B$3-AB3)/(AB4-AB3),IF($B$3&lt;AB5,255,IF($B$3&lt;AB6,255*(AB6-$B$3)/(AB6-AB5),0))))</f>
-        <v>22.767857142857142</v>
+        <v>0</v>
       </c>
       <c r="O3" s="2">
         <f>IF($B$3&lt;AC3,0,IF($B$3&lt;AC4,255*($B$3-AC3)/(AC4-AC3),IF($B$3&lt;AC5,255,IF($B$3&lt;AC6,255*(AC6-$B$3)/(AC6-AC5),0))))</f>
-        <v>255</v>
+        <v>86.517857142857139</v>
       </c>
       <c r="P3" s="2">
         <f>IF($B$3&lt;AD3,0,IF($B$3&lt;AD4,255*($B$3-AD3)/(AD4-AD3),IF($B$3&lt;AD5,255,IF($B$3&lt;AD6,255*(AD6-$B$3)/(AD6-AD5),0))))</f>
-        <v>0</v>
+        <v>197.41935483870967</v>
       </c>
       <c r="R3" t="s">
         <v>11</v>
@@ -954,15 +954,15 @@
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f>MAX(MIN(E3,H3),MIN(E3,I3),MIN(F3,H3))</f>
-        <v>71.83098591549296</v>
+        <v>48.571428571428569</v>
       </c>
       <c r="B8" s="1">
         <f>MAX(MIN(G3,H3),MIN(F3,I3),MIN(E3,J3))</f>
-        <v>255</v>
+        <v>122.11267605633803</v>
       </c>
       <c r="C8" s="1">
         <f>MAX(MIN(G3,I3),MIN(G3,J3),MIN(F3,J3))</f>
-        <v>0</v>
+        <v>208.63636363636363</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
@@ -976,7 +976,7 @@
       <c r="C9" s="11"/>
       <c r="F9" s="13">
         <f>(A14*(A8+A11)+B14*(B8+B11)+C14*(C11+C8))/(A8+A11+B8+B11+C8+C11)</f>
-        <v>107.28535058873449</v>
+        <v>189.06813584290444</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
@@ -999,11 +999,11 @@
       </c>
       <c r="B11" s="1">
         <f>MAX(MIN(K3,P3),MIN(L3,O3),MIN(M3,N3))</f>
-        <v>255</v>
+        <v>86.517857142857139</v>
       </c>
       <c r="C11" s="1">
         <f>MAX(MIN(L3,P3),MIN(M3,O3),MIN(M3,P3))</f>
-        <v>0</v>
+        <v>197.41935483870967</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
versao final final com 90 MHZ
</commit_message>
<xml_diff>
--- a/Planilhas Excel/Conferencia_de_valores.xlsx
+++ b/Planilhas Excel/Conferencia_de_valores.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3beaf518c581d7d9/Documentos/GitHub/Fuzzy_Logic_2_Controller/Planilhas Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{E7D119CA-9AE4-4C47-BE3C-22F746B05797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68D97908-D838-493D-80F2-F30BA6CC3C0D}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{E7D119CA-9AE4-4C47-BE3C-22F746B05797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A36BF00B-75DA-42BB-949F-6266D7052765}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="3660" yWindow="2475" windowWidth="21600" windowHeight="11295" xr2:uid="{377A5F18-558A-4A8F-B21A-CB5653200D67}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,6 +39,21 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="22">
   <si>
+    <t>Entradas</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>Entrada 1</t>
+  </si>
+  <si>
+    <t>Entrada 2</t>
+  </si>
+  <si>
     <t>MF1</t>
   </si>
   <si>
@@ -57,21 +72,6 @@
     <t>MF6</t>
   </si>
   <si>
-    <t>UP</t>
-  </si>
-  <si>
-    <t>LOW</t>
-  </si>
-  <si>
-    <t>Entradas</t>
-  </si>
-  <si>
-    <t>Entrada 1</t>
-  </si>
-  <si>
-    <t>Entrada 2</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -84,13 +84,13 @@
     <t>D</t>
   </si>
   <si>
+    <t>uN</t>
+  </si>
+  <si>
     <t>uZ</t>
   </si>
   <si>
     <t>uP</t>
-  </si>
-  <si>
-    <t>uN</t>
   </si>
   <si>
     <t>saída</t>
@@ -109,7 +109,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,12 +278,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -571,7 +567,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -585,20 +581,20 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="17" width="9.140625" style="1"/>
     <col min="18" max="30" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="31" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30">
       <c r="A1" s="11" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" s="11"/>
       <c r="E1" s="14" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F1" s="14"/>
       <c r="G1" s="14"/>
@@ -606,7 +602,7 @@
       <c r="I1" s="14"/>
       <c r="J1" s="15"/>
       <c r="K1" s="16" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
@@ -615,7 +611,7 @@
       <c r="P1" s="14"/>
       <c r="R1"/>
       <c r="S1" s="10" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="T1" s="10"/>
       <c r="U1" s="10"/>
@@ -623,7 +619,7 @@
       <c r="W1" s="10"/>
       <c r="X1" s="10"/>
       <c r="Y1" s="10" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="Z1" s="10"/>
       <c r="AA1" s="10"/>
@@ -631,141 +627,141 @@
       <c r="AC1" s="10"/>
       <c r="AD1" s="10"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30">
       <c r="A2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="J2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>0</v>
-      </c>
       <c r="L2" s="5" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R2"/>
       <c r="S2" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="X2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Y2" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="Z2" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30">
       <c r="A3" s="1">
-        <v>102</v>
+        <v>160</v>
       </c>
       <c r="B3" s="1">
-        <v>216</v>
+        <v>80</v>
       </c>
       <c r="E3" s="2">
         <f>IF($A$3&lt;S3,0,IF($A$3&lt;S4,255*($A$3-S3)/(S4-S3),IF($A$3&lt;S5,255,IF($A$3&lt;S6,255*(S6-$A$3)/(S6-S5),0))))</f>
-        <v>48.571428571428569</v>
+        <v>0</v>
       </c>
       <c r="F3" s="2">
         <f>IF($A$3&lt;T3,0,IF($A$3&lt;T4,255*($A$3-T3)/(T4-T3),IF($A$3&lt;T5,255,IF($A$3&lt;T6,255*(T6-$A$3)/(T6-T5),0))))</f>
-        <v>255</v>
+        <v>229.13043478260869</v>
       </c>
       <c r="G3" s="2">
         <f>IF($A$3&lt;U3,0,IF($A$3&lt;U4,255*($A$3-U3)/(U4-U3),IF($A$3&lt;U5,255,IF($A$3&lt;U6,255*(U6-$A$3)/(U6-U5),0))))</f>
-        <v>0</v>
+        <v>175.57377049180329</v>
       </c>
       <c r="H3" s="2">
         <f>IF($B$3&lt;V3,0,IF($B$3&lt;V4,255*($B$3-V3)/(V4-V3),IF($B$3&lt;V5,255,IF($B$3&lt;V6,255*(V6-$B$3)/(V6-V5),0))))</f>
-        <v>0</v>
+        <v>244.22535211267606</v>
       </c>
       <c r="I3" s="2">
         <f>IF($B$3&lt;W3,0,IF($B$3&lt;W4,255*($B$3-W3)/(W4-W3),IF($B$3&lt;W5,255,IF($B$3&lt;W6,255*(W6-$B$3)/(W6-W5),0))))</f>
-        <v>122.11267605633803</v>
+        <v>175.98591549295776</v>
       </c>
       <c r="J3" s="4">
         <f>IF($B$3&lt;X3,0,IF($B$3&lt;X4,255*($B$3-X3)/(X4-X3),IF($B$3&lt;X5,255,IF($B$3&lt;X6,255*(X6-$B$3)/(X6-X5),0))))</f>
-        <v>208.63636363636363</v>
+        <v>0</v>
       </c>
       <c r="K3" s="3">
         <f>IF($A$3&lt;Y3,0,IF($A$3&lt;Y4,255*($A$3-Y3)/(Y4-Y3),IF($A$3&lt;Y5,255,IF($A$3&lt;Y6,255*(Y6-$A$3)/(Y6-Y5),0))))</f>
-        <v>22.767857142857142</v>
+        <v>0</v>
       </c>
       <c r="L3" s="2">
         <f>IF($A$3&lt;Z3,0,IF($A$3&lt;Z4,255*($A$3-Z3)/(Z4-Z3),IF($A$3&lt;Z5,255,IF($A$3&lt;Z6,255*(Z6-$A$3)/(Z6-Z5),0))))</f>
-        <v>255</v>
+        <v>223.125</v>
       </c>
       <c r="M3" s="2">
         <f>IF($A$3&lt;AA3,0,IF($A$3&lt;AA4,255*($A$3-AA3)/(AA4-AA3),IF($A$3&lt;AA5,255,IF($A$3&lt;AA6,255*(AA6-$A$3)/(AA6-AA5),0))))</f>
-        <v>0</v>
+        <v>165.27777777777777</v>
       </c>
       <c r="N3" s="2">
         <f>IF($B$3&lt;AB3,0,IF($B$3&lt;AB4,255*($B$3-AB3)/(AB4-AB3),IF($B$3&lt;AB5,255,IF($B$3&lt;AB6,255*(AB6-$B$3)/(AB6-AB5),0))))</f>
-        <v>0</v>
+        <v>241.33928571428572</v>
       </c>
       <c r="O3" s="2">
         <f>IF($B$3&lt;AC3,0,IF($B$3&lt;AC4,255*($B$3-AC3)/(AC4-AC3),IF($B$3&lt;AC5,255,IF($B$3&lt;AC6,255*(AC6-$B$3)/(AC6-AC5),0))))</f>
-        <v>86.517857142857139</v>
+        <v>154.82142857142858</v>
       </c>
       <c r="P3" s="2">
         <f>IF($B$3&lt;AD3,0,IF($B$3&lt;AD4,255*($B$3-AD3)/(AD4-AD3),IF($B$3&lt;AD5,255,IF($B$3&lt;AD6,255*(AD6-$B$3)/(AD6-AD5),0))))</f>
-        <v>197.41935483870967</v>
+        <v>0</v>
       </c>
       <c r="R3" t="s">
         <v>11</v>
@@ -807,7 +803,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30">
       <c r="R4" t="s">
         <v>12</v>
       </c>
@@ -848,7 +844,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="R5" t="s">
         <v>13</v>
       </c>
@@ -889,9 +885,9 @@
         <v>254</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30">
       <c r="A6" s="11" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -935,15 +931,15 @@
         <v>255</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30">
       <c r="A7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>18</v>
@@ -951,62 +947,62 @@
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30">
       <c r="A8" s="1">
         <f>MAX(MIN(E3,H3),MIN(E3,I3),MIN(F3,H3))</f>
-        <v>48.571428571428569</v>
+        <v>229.13043478260869</v>
       </c>
       <c r="B8" s="1">
         <f>MAX(MIN(G3,H3),MIN(F3,I3),MIN(E3,J3))</f>
-        <v>122.11267605633803</v>
+        <v>175.98591549295776</v>
       </c>
       <c r="C8" s="1">
         <f>MAX(MIN(G3,I3),MIN(G3,J3),MIN(F3,J3))</f>
-        <v>208.63636363636363</v>
+        <v>175.57377049180329</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:30" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" ht="31.5">
       <c r="A9" s="11" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="F9" s="13">
         <f>(A14*(A8+A11)+B14*(B8+B11)+C14*(C11+C8))/(A8+A11+B8+B11+C8+C11)</f>
-        <v>189.06813584290444</v>
+        <v>113.63243795448126</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30">
       <c r="A10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:30">
       <c r="A11" s="1">
         <f>MAX(MIN(K3,N3),MIN(K3,O3),MIN(L3,N3))</f>
-        <v>22.767857142857142</v>
+        <v>223.125</v>
       </c>
       <c r="B11" s="1">
         <f>MAX(MIN(K3,P3),MIN(L3,O3),MIN(M3,N3))</f>
-        <v>86.517857142857139</v>
+        <v>165.27777777777777</v>
       </c>
       <c r="C11" s="1">
         <f>MAX(MIN(L3,P3),MIN(M3,O3),MIN(M3,P3))</f>
-        <v>197.41935483870967</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+        <v>154.82142857142858</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1017,7 +1013,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -1053,11 +1049,11 @@
       <selection sqref="A1:M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="B1" s="10" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -1065,7 +1061,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="H1" s="10" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
@@ -1073,45 +1069,45 @@
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="I2" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1152,7 +1148,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1193,7 +1189,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1234,7 +1230,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>14</v>
       </c>

</xml_diff>